<commit_message>
Upload Personal Finance Tracker
</commit_message>
<xml_diff>
--- a/Personal Expense Tracker - Troy Fleming.xlsx
+++ b/Personal Expense Tracker - Troy Fleming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tress\Troy - Coding Temple\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51495E24-6863-4E3F-9B24-6B60342E68CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C667FC-B3FB-452B-BAE5-102CD8EA2ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4CCB0D4B-2213-48E7-BDC1-E1AA6B552E49}"/>
   </bookViews>
@@ -279,7 +279,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -324,6 +324,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -589,7 +601,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$7:$D$10</c:f>
+              <c:f>Sheet1!$D$26:$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -609,7 +621,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$10</c:f>
+              <c:f>Sheet1!$F$26:$F$29</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1600,7 +1612,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,13 +1673,6 @@
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="10">
-        <f>$B$12</f>
-        <v>1752.3400000000001</v>
-      </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1680,13 +1685,6 @@
         <f>($B8/$B$2)</f>
         <v>0.45714285714285713</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="10">
-        <f>B21</f>
-        <v>174.8</v>
-      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1699,13 +1697,6 @@
         <f>($B9/$B$2)</f>
         <v>4.2542857142857148E-3</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="10">
-        <f>B33</f>
-        <v>1018.97</v>
-      </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1717,13 +1708,6 @@
       <c r="C10" s="8">
         <f>($B10/$B$2)</f>
         <v>3.9271428571428568E-2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="10">
-        <f>$B$37</f>
-        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1857,13 +1841,13 @@
         <f t="shared" si="0"/>
         <v>1.1425714285714286E-2</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="19"/>
+      <c r="D26" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="20"/>
       <c r="F26" s="10">
-        <f>SUM(B12,B21,B33,B37)</f>
-        <v>3446.11</v>
+        <f>$B$12</f>
+        <v>1752.3400000000001</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1877,13 +1861,13 @@
         <f t="shared" si="0"/>
         <v>1.1428571428571429E-2</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="9">
-        <f>$F$2-$F$26</f>
-        <v>53.889999999999873</v>
+      <c r="D27" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="10">
+        <f>B21</f>
+        <v>174.8</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1897,6 +1881,14 @@
         <f t="shared" si="0"/>
         <v>2.1428571428571429E-2</v>
       </c>
+      <c r="D28" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="10">
+        <f>B33</f>
+        <v>1018.97</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -1909,6 +1901,14 @@
         <f t="shared" si="0"/>
         <v>6.2857142857142861E-2</v>
       </c>
+      <c r="D29" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="10">
+        <f>$B$37</f>
+        <v>500</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -1933,6 +1933,24 @@
         <f t="shared" si="0"/>
         <v>6.8514285714285717E-3</v>
       </c>
+      <c r="D31" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="10">
+        <f>SUM(B12,B21,B33,B37)</f>
+        <v>3446.11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="9">
+        <f>$F$2-$F$31</f>
+        <v>53.889999999999873</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -1972,17 +1990,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
-  <conditionalFormatting sqref="F26">
+  <conditionalFormatting sqref="F31">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
+  <conditionalFormatting sqref="F32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1994,7 +2016,7 @@
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B33:B34 B20:B24 B11:B15" xr:uid="{F27CFDF2-F1A1-4EF7-997C-4B2AB5E6D5AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27" xr:uid="{93DBDBCB-D09E-4C5A-8D6E-50CA7A1000C3}"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F32" xr:uid="{93DBDBCB-D09E-4C5A-8D6E-50CA7A1000C3}"/>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mortage / Rent Payment" prompt="How much do you pay for your mortgage or rent each month?" sqref="B8" xr:uid="{815109E1-8086-4A34-8851-32A02E841D6A}">
       <formula1>0</formula1>
     </dataValidation>

</xml_diff>